<commit_message>
:art: - label calculations - highlight differences sa in email text
</commit_message>
<xml_diff>
--- a/projects/2025_NJSTAP/Exceedance/tabulated/Exceedance_table_NJSTAP_praveen_new.xlsx
+++ b/projects/2025_NJSTAP/Exceedance/tabulated/Exceedance_table_NJSTAP_praveen_new.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pk695/werk.M2/FACTS_dev/facts.postprocess.pub/projects/2025_NJSTAP/Exceedance/tabulated/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/geekBoi_18/werk/amarel/scratch:pk695/NJ_STAP_report/notebooks/xcdance/_print.xcdance.table_xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F94A0D8-1131-2640-A3D2-141C60A7C0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BC2DC0-9720-5740-8F0A-733D726A8A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32740" yWindow="-14800" windowWidth="29920" windowHeight="18660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-46840" yWindow="-18720" windowWidth="29920" windowHeight="18660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SANDY_HOOK" sheetId="9" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="PHILADELPHIA" sheetId="7" r:id="rId3"/>
     <sheet name="NYC" sheetId="6" r:id="rId4"/>
     <sheet name="Atlantic City" sheetId="2" r:id="rId5"/>
-    <sheet name="NJSTAP.Coastal" sheetId="12" r:id="rId6"/>
+    <sheet name="NJSTAP.Coastal" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="252">
   <si>
     <t>2042 (2027,2032, 2060,2081)</t>
   </si>
@@ -2853,13 +2853,37 @@
       </rPr>
       <t xml:space="preserve">to exceed 5 ft before </t>
     </r>
+  </si>
+  <si>
+    <t>xls calculation 1</t>
+  </si>
+  <si>
+    <t>xls calculation 2</t>
+  </si>
+  <si>
+    <t>xls calculation 3</t>
+  </si>
+  <si>
+    <t>xls calculation 4</t>
+  </si>
+  <si>
+    <t>xls calculation 5</t>
+  </si>
+  <si>
+    <t>xls calculation 6</t>
+  </si>
+  <si>
+    <t>xls calculation 7</t>
+  </si>
+  <si>
+    <t>xls calculation 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2897,6 +2921,22 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFA02B93"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2937,7 +2977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2976,18 +3016,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4637,11 +4681,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E6466B-045C-704A-823D-1F35C5F94911}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71CD506C-7B6F-1F41-8B2A-FA4AF67E1BCF}">
   <dimension ref="A3:AC138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AA139" sqref="AA139:AA140"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="U69" sqref="U69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4662,37 +4706,37 @@
       <c r="A3" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="18" t="s">
+      <c r="N3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="18" t="s">
+      <c r="T3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
       <c r="Y3" s="8"/>
       <c r="AA3" s="1"/>
     </row>
@@ -5437,37 +5481,37 @@
       <c r="A21" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="18" t="s">
+      <c r="N21" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
       <c r="S21" s="8"/>
-      <c r="T21" s="18" t="s">
+      <c r="T21" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="19"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
       <c r="Y21" s="8"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
@@ -6205,37 +6249,37 @@
       <c r="A38" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="18" t="s">
+      <c r="H38" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
       <c r="M38" s="8"/>
-      <c r="N38" s="18" t="s">
+      <c r="N38" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
       <c r="S38" s="8"/>
-      <c r="T38" s="18" t="s">
+      <c r="T38" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+      <c r="W38" s="17"/>
+      <c r="X38" s="17"/>
       <c r="Y38" s="8"/>
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
@@ -6971,18 +7015,27 @@
       <c r="X51" s="8"/>
       <c r="Y51" s="8"/>
     </row>
+    <row r="55" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="I55" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="J55" s="22"/>
+    </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="18" t="s">
         <v>236</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
-      <c r="H56" s="16" t="s">
+      <c r="H56" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="I56" s="16"/>
+      <c r="I56" s="19"/>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
@@ -6993,7 +7046,7 @@
       <c r="Q56" s="7"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A57" s="20"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7">
@@ -7004,13 +7057,13 @@
         <f>MAX(E5:E7,E12:E14,E23:E25,E30:E32,E40:E42,E47:E49)</f>
         <v>2056</v>
       </c>
-      <c r="H57" s="16"/>
-      <c r="I57" s="16"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
       <c r="J57" s="7">
         <f>MIN(J5,J23,J40)</f>
         <v>2091</v>
       </c>
-      <c r="K57" s="7">
+      <c r="K57" s="13">
         <f>MAX(K5,K23,K40)</f>
         <v>2224</v>
       </c>
@@ -7028,13 +7081,13 @@
       </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A58" s="20"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
       <c r="L58" s="7"/>
@@ -7045,13 +7098,13 @@
       <c r="Q58" s="7"/>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A59" s="20"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="16"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
       <c r="L59" s="7"/>
@@ -7062,13 +7115,13 @@
       <c r="Q59" s="7"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A60" s="20"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="16"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
@@ -7079,13 +7132,13 @@
       <c r="Q60" s="7"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A61" s="20"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="16"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
@@ -7096,13 +7149,13 @@
       <c r="Q61" s="7"/>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A62" s="20"/>
+      <c r="A62" s="18"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
-      <c r="H62" s="16"/>
-      <c r="I62" s="16"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
       <c r="L62" s="7"/>
@@ -7113,13 +7166,13 @@
       <c r="Q62" s="7"/>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A63" s="20"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
       <c r="L63" s="7"/>
@@ -7130,13 +7183,13 @@
       <c r="Q63" s="7"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A64" s="20"/>
+      <c r="A64" s="18"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
       <c r="L64" s="7"/>
@@ -7147,8 +7200,8 @@
       <c r="Q64" s="7"/>
     </row>
     <row r="65" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
       <c r="L65" s="7"/>
@@ -7159,8 +7212,8 @@
       <c r="Q65" s="7"/>
     </row>
     <row r="66" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
       <c r="L66" s="7"/>
@@ -7171,8 +7224,8 @@
       <c r="Q66" s="7"/>
     </row>
     <row r="67" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H67" s="16"/>
-      <c r="I67" s="16"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
       <c r="L67" s="7"/>
@@ -7182,11 +7235,17 @@
       <c r="P67" s="7"/>
       <c r="Q67" s="7"/>
     </row>
+    <row r="71" spans="8:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="I71" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="J71" s="22"/>
+    </row>
     <row r="72" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H72" s="16" t="s">
+      <c r="H72" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="I72" s="16"/>
+      <c r="I72" s="19"/>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
@@ -7197,8 +7256,8 @@
       <c r="Q72" s="7"/>
     </row>
     <row r="73" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H73" s="16"/>
-      <c r="I73" s="16"/>
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
       <c r="J73" s="7">
         <f>MIN(J6,J24,J41)</f>
         <v>2082</v>
@@ -7215,14 +7274,14 @@
         <f>MIN(P6,P24,P41)</f>
         <v>2124</v>
       </c>
-      <c r="Q73" s="7">
+      <c r="Q73" s="13">
         <f>MAX(Q6,Q24,Q41)</f>
         <v>2269</v>
       </c>
     </row>
     <row r="74" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H74" s="16"/>
-      <c r="I74" s="16"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
@@ -7233,8 +7292,8 @@
       <c r="Q74" s="7"/>
     </row>
     <row r="75" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
@@ -7245,8 +7304,8 @@
       <c r="Q75" s="7"/>
     </row>
     <row r="76" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H76" s="16"/>
-      <c r="I76" s="16"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
@@ -7257,8 +7316,8 @@
       <c r="Q76" s="7"/>
     </row>
     <row r="77" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H77" s="16"/>
-      <c r="I77" s="16"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
@@ -7269,8 +7328,8 @@
       <c r="Q77" s="7"/>
     </row>
     <row r="78" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H78" s="16"/>
-      <c r="I78" s="16"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
@@ -7281,8 +7340,8 @@
       <c r="Q78" s="7"/>
     </row>
     <row r="79" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H79" s="16"/>
-      <c r="I79" s="16"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
@@ -7293,8 +7352,8 @@
       <c r="Q79" s="7"/>
     </row>
     <row r="80" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H80" s="16"/>
-      <c r="I80" s="16"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
@@ -7305,8 +7364,8 @@
       <c r="Q80" s="7"/>
     </row>
     <row r="81" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H81" s="16"/>
-      <c r="I81" s="16"/>
+      <c r="H81" s="19"/>
+      <c r="I81" s="19"/>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
@@ -7317,8 +7376,8 @@
       <c r="Q81" s="7"/>
     </row>
     <row r="82" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H82" s="16"/>
-      <c r="I82" s="16"/>
+      <c r="H82" s="19"/>
+      <c r="I82" s="19"/>
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
       <c r="L82" s="7"/>
@@ -7329,8 +7388,8 @@
       <c r="Q82" s="7"/>
     </row>
     <row r="83" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H83" s="16"/>
-      <c r="I83" s="16"/>
+      <c r="H83" s="19"/>
+      <c r="I83" s="19"/>
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
       <c r="L83" s="7"/>
@@ -7340,11 +7399,17 @@
       <c r="P83" s="7"/>
       <c r="Q83" s="7"/>
     </row>
+    <row r="86" spans="6:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="I86" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="J86" s="22"/>
+    </row>
     <row r="87" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H87" s="16" t="s">
+      <c r="H87" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="I87" s="16"/>
+      <c r="I87" s="19"/>
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
       <c r="L87" s="7"/>
@@ -7355,8 +7420,8 @@
       <c r="Q87" s="7"/>
     </row>
     <row r="88" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H88" s="16"/>
-      <c r="I88" s="16"/>
+      <c r="H88" s="19"/>
+      <c r="I88" s="19"/>
       <c r="J88" s="7">
         <f>MIN(J7,J25,J42)</f>
         <v>2078</v>
@@ -7373,14 +7438,14 @@
         <f>MIN(P7,P25,P42)</f>
         <v>2112</v>
       </c>
-      <c r="Q88" s="7">
+      <c r="Q88" s="13">
         <f>MAX(Q7,Q25,Q42)</f>
         <v>2197</v>
       </c>
     </row>
     <row r="89" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H89" s="16"/>
-      <c r="I89" s="16"/>
+      <c r="H89" s="19"/>
+      <c r="I89" s="19"/>
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
       <c r="L89" s="7"/>
@@ -7393,8 +7458,8 @@
     <row r="90" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
-      <c r="H90" s="16"/>
-      <c r="I90" s="16"/>
+      <c r="H90" s="19"/>
+      <c r="I90" s="19"/>
       <c r="J90" s="11"/>
       <c r="K90" s="7"/>
       <c r="L90" s="7"/>
@@ -7408,8 +7473,8 @@
     <row r="91" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
-      <c r="H91" s="16"/>
-      <c r="I91" s="16"/>
+      <c r="H91" s="19"/>
+      <c r="I91" s="19"/>
       <c r="J91" s="11"/>
       <c r="K91" s="7"/>
       <c r="L91" s="7"/>
@@ -7423,8 +7488,8 @@
     <row r="92" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
-      <c r="H92" s="16"/>
-      <c r="I92" s="16"/>
+      <c r="H92" s="19"/>
+      <c r="I92" s="19"/>
       <c r="J92" s="11"/>
       <c r="K92" s="7"/>
       <c r="L92" s="7"/>
@@ -7438,8 +7503,8 @@
     <row r="93" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F93" s="5"/>
       <c r="G93" s="4"/>
-      <c r="H93" s="16"/>
-      <c r="I93" s="16"/>
+      <c r="H93" s="19"/>
+      <c r="I93" s="19"/>
       <c r="J93" s="11"/>
       <c r="K93" s="7"/>
       <c r="L93" s="7"/>
@@ -7453,8 +7518,8 @@
     <row r="94" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F94" s="5"/>
       <c r="G94" s="4"/>
-      <c r="H94" s="16"/>
-      <c r="I94" s="16"/>
+      <c r="H94" s="19"/>
+      <c r="I94" s="19"/>
       <c r="J94" s="11"/>
       <c r="K94" s="7"/>
       <c r="L94" s="7"/>
@@ -7466,8 +7531,8 @@
       <c r="S94" s="4"/>
     </row>
     <row r="95" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H95" s="16"/>
-      <c r="I95" s="16"/>
+      <c r="H95" s="19"/>
+      <c r="I95" s="19"/>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
       <c r="L95" s="7"/>
@@ -7478,8 +7543,8 @@
       <c r="Q95" s="7"/>
     </row>
     <row r="96" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H96" s="16"/>
-      <c r="I96" s="16"/>
+      <c r="H96" s="19"/>
+      <c r="I96" s="19"/>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
       <c r="L96" s="7"/>
@@ -7490,8 +7555,8 @@
       <c r="Q96" s="7"/>
     </row>
     <row r="97" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H97" s="16"/>
-      <c r="I97" s="16"/>
+      <c r="H97" s="19"/>
+      <c r="I97" s="19"/>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
       <c r="L97" s="7"/>
@@ -7502,8 +7567,8 @@
       <c r="Q97" s="7"/>
     </row>
     <row r="98" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H98" s="16"/>
-      <c r="I98" s="16"/>
+      <c r="H98" s="19"/>
+      <c r="I98" s="19"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
       <c r="L98" s="7"/>
@@ -7513,17 +7578,27 @@
       <c r="P98" s="7"/>
       <c r="Q98" s="7"/>
     </row>
+    <row r="101" spans="8:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="I101" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="J101" s="22"/>
+      <c r="P101" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q101" s="22"/>
+    </row>
     <row r="102" spans="8:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
-      <c r="K102" s="17" t="s">
+      <c r="K102" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="L102" s="17"/>
-      <c r="P102" s="17" t="s">
+      <c r="L102" s="20"/>
+      <c r="P102" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="Q102" s="17"/>
+      <c r="Q102" s="20"/>
     </row>
     <row r="103" spans="8:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I103" s="7">
@@ -7531,193 +7606,212 @@
         <v>2060</v>
       </c>
       <c r="J103" s="7"/>
-      <c r="K103" s="17"/>
-      <c r="L103" s="17"/>
+      <c r="K103" s="20"/>
+      <c r="L103" s="20"/>
       <c r="O103">
         <f>MIN(O5,O12,O23,O30,O40,O47)</f>
         <v>2099</v>
       </c>
-      <c r="P103" s="17"/>
-      <c r="Q103" s="17"/>
+      <c r="P103" s="20"/>
+      <c r="Q103" s="20"/>
     </row>
     <row r="104" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
-      <c r="K104" s="17"/>
-      <c r="L104" s="17"/>
-      <c r="P104" s="17"/>
-      <c r="Q104" s="17"/>
+      <c r="K104" s="20"/>
+      <c r="L104" s="20"/>
+      <c r="P104" s="20"/>
+      <c r="Q104" s="20"/>
     </row>
     <row r="105" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
-      <c r="K105" s="17"/>
-      <c r="L105" s="17"/>
-      <c r="P105" s="17"/>
-      <c r="Q105" s="17"/>
+      <c r="K105" s="20"/>
+      <c r="L105" s="20"/>
+      <c r="P105" s="20"/>
+      <c r="Q105" s="20"/>
     </row>
     <row r="106" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
-      <c r="K106" s="17"/>
-      <c r="L106" s="17"/>
-      <c r="P106" s="17"/>
-      <c r="Q106" s="17"/>
+      <c r="K106" s="20"/>
+      <c r="L106" s="20"/>
+      <c r="P106" s="20"/>
+      <c r="Q106" s="20"/>
     </row>
     <row r="107" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
-      <c r="K107" s="17"/>
-      <c r="L107" s="17"/>
-      <c r="P107" s="17"/>
-      <c r="Q107" s="17"/>
+      <c r="K107" s="20"/>
+      <c r="L107" s="20"/>
+      <c r="P107" s="20"/>
+      <c r="Q107" s="20"/>
     </row>
     <row r="108" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
-      <c r="K108" s="17"/>
-      <c r="L108" s="17"/>
-      <c r="P108" s="17"/>
-      <c r="Q108" s="17"/>
+      <c r="K108" s="20"/>
+      <c r="L108" s="20"/>
+      <c r="P108" s="20"/>
+      <c r="Q108" s="20"/>
     </row>
     <row r="109" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
-      <c r="K109" s="17"/>
-      <c r="L109" s="17"/>
-      <c r="P109" s="17"/>
-      <c r="Q109" s="17"/>
+      <c r="K109" s="20"/>
+      <c r="L109" s="20"/>
+      <c r="P109" s="20"/>
+      <c r="Q109" s="20"/>
     </row>
     <row r="110" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
-      <c r="K110" s="17"/>
-      <c r="L110" s="17"/>
-      <c r="P110" s="17"/>
-      <c r="Q110" s="17"/>
+      <c r="K110" s="20"/>
+      <c r="L110" s="20"/>
+      <c r="P110" s="20"/>
+      <c r="Q110" s="20"/>
     </row>
     <row r="111" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
-      <c r="K111" s="17"/>
-      <c r="L111" s="17"/>
-      <c r="P111" s="17"/>
-      <c r="Q111" s="17"/>
+      <c r="K111" s="20"/>
+      <c r="L111" s="20"/>
+      <c r="P111" s="20"/>
+      <c r="Q111" s="20"/>
+    </row>
+    <row r="115" spans="15:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="P115" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q115" s="22"/>
     </row>
     <row r="116" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P116" s="17" t="s">
+      <c r="P116" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="Q116" s="17"/>
+      <c r="Q116" s="20"/>
     </row>
     <row r="117" spans="15:17" x14ac:dyDescent="0.2">
       <c r="O117">
         <f>MIN(O6,O13,O24,O41,O48,O31)</f>
         <v>2088</v>
       </c>
-      <c r="P117" s="17"/>
-      <c r="Q117" s="17"/>
+      <c r="P117" s="20"/>
+      <c r="Q117" s="20"/>
     </row>
     <row r="118" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P118" s="17"/>
-      <c r="Q118" s="17"/>
+      <c r="P118" s="20"/>
+      <c r="Q118" s="20"/>
     </row>
     <row r="119" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P119" s="17"/>
-      <c r="Q119" s="17"/>
+      <c r="P119" s="20"/>
+      <c r="Q119" s="20"/>
     </row>
     <row r="120" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P120" s="17"/>
-      <c r="Q120" s="17"/>
+      <c r="P120" s="20"/>
+      <c r="Q120" s="20"/>
     </row>
     <row r="121" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P121" s="17"/>
-      <c r="Q121" s="17"/>
+      <c r="P121" s="20"/>
+      <c r="Q121" s="20"/>
     </row>
     <row r="122" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P122" s="17"/>
-      <c r="Q122" s="17"/>
+      <c r="P122" s="20"/>
+      <c r="Q122" s="20"/>
     </row>
     <row r="123" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P123" s="17"/>
-      <c r="Q123" s="17"/>
+      <c r="P123" s="20"/>
+      <c r="Q123" s="20"/>
     </row>
     <row r="124" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P124" s="17"/>
-      <c r="Q124" s="17"/>
+      <c r="P124" s="20"/>
+      <c r="Q124" s="20"/>
     </row>
     <row r="125" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P125" s="17"/>
-      <c r="Q125" s="17"/>
+      <c r="P125" s="20"/>
+      <c r="Q125" s="20"/>
+    </row>
+    <row r="128" spans="15:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="P128" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q128" s="22"/>
     </row>
     <row r="129" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P129" s="17" t="s">
+      <c r="P129" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="Q129" s="17"/>
+      <c r="Q129" s="20"/>
     </row>
     <row r="130" spans="15:17" x14ac:dyDescent="0.2">
       <c r="O130">
         <f>MIN(O7,O14,O25,O32,O42,O49)</f>
         <v>2081</v>
       </c>
-      <c r="P130" s="17"/>
-      <c r="Q130" s="17"/>
+      <c r="P130" s="20"/>
+      <c r="Q130" s="20"/>
     </row>
     <row r="131" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P131" s="17"/>
-      <c r="Q131" s="17"/>
+      <c r="P131" s="20"/>
+      <c r="Q131" s="20"/>
     </row>
     <row r="132" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P132" s="17"/>
-      <c r="Q132" s="17"/>
+      <c r="P132" s="20"/>
+      <c r="Q132" s="20"/>
     </row>
     <row r="133" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P133" s="17"/>
-      <c r="Q133" s="17"/>
+      <c r="P133" s="20"/>
+      <c r="Q133" s="20"/>
     </row>
     <row r="134" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P134" s="17"/>
-      <c r="Q134" s="17"/>
+      <c r="P134" s="20"/>
+      <c r="Q134" s="20"/>
     </row>
     <row r="135" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P135" s="17"/>
-      <c r="Q135" s="17"/>
+      <c r="P135" s="20"/>
+      <c r="Q135" s="20"/>
     </row>
     <row r="136" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P136" s="17"/>
-      <c r="Q136" s="17"/>
+      <c r="P136" s="20"/>
+      <c r="Q136" s="20"/>
     </row>
     <row r="137" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P137" s="17"/>
-      <c r="Q137" s="17"/>
+      <c r="P137" s="20"/>
+      <c r="Q137" s="20"/>
     </row>
     <row r="138" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P138" s="17"/>
-      <c r="Q138" s="17"/>
+      <c r="P138" s="20"/>
+      <c r="Q138" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="27">
+    <mergeCell ref="K102:L111"/>
+    <mergeCell ref="P102:Q111"/>
+    <mergeCell ref="P115:Q115"/>
+    <mergeCell ref="P116:Q125"/>
+    <mergeCell ref="P128:Q128"/>
+    <mergeCell ref="P129:Q138"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="H72:I83"/>
+    <mergeCell ref="I86:J86"/>
+    <mergeCell ref="H87:I98"/>
+    <mergeCell ref="I101:J101"/>
+    <mergeCell ref="P101:Q101"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="N38:R38"/>
+    <mergeCell ref="T38:X38"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="A56:A64"/>
+    <mergeCell ref="H56:I67"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="N3:R3"/>
     <mergeCell ref="T3:X3"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="H21:L21"/>
     <mergeCell ref="N21:R21"/>
     <mergeCell ref="T21:X21"/>
-    <mergeCell ref="A56:A64"/>
-    <mergeCell ref="H56:I67"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="P129:Q138"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="N38:R38"/>
-    <mergeCell ref="T38:X38"/>
-    <mergeCell ref="H72:I83"/>
-    <mergeCell ref="H87:I98"/>
-    <mergeCell ref="K102:L111"/>
-    <mergeCell ref="P102:Q111"/>
-    <mergeCell ref="P116:Q125"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
:heavy_plus_sign: Atlantic city sheet
</commit_message>
<xml_diff>
--- a/projects/2025_NJSTAP/Exceedance/tabulated/Exceedance_table_NJSTAP_praveen_new.xlsx
+++ b/projects/2025_NJSTAP/Exceedance/tabulated/Exceedance_table_NJSTAP_praveen_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/geekBoi_18/werk/amarel/scratch:pk695/NJ_STAP_report/notebooks/xcdance/_print.xcdance.table_xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BC2DC0-9720-5740-8F0A-733D726A8A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E496600-C2AC-AE42-BF42-0C36328F42E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46840" yWindow="-18720" windowWidth="29920" windowHeight="18660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-46840" yWindow="-18720" windowWidth="29920" windowHeight="18660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SANDY_HOOK" sheetId="9" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="NYC" sheetId="6" r:id="rId4"/>
     <sheet name="Atlantic City" sheetId="2" r:id="rId5"/>
     <sheet name="NJSTAP.Coastal" sheetId="13" r:id="rId6"/>
+    <sheet name="NJSTAP_AtlanticCity" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="252">
   <si>
     <t>2042 (2027,2032, 2060,2081)</t>
   </si>
@@ -2977,7 +2978,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3015,7 +3016,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3023,15 +3034,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3351,19 +3355,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3616,19 +3620,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3877,19 +3881,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -4138,19 +4142,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -4403,19 +4407,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -4684,7 +4688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71CD506C-7B6F-1F41-8B2A-FA4AF67E1BCF}">
   <dimension ref="A3:AC138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="U69" sqref="U69"/>
     </sheetView>
   </sheetViews>
@@ -4706,37 +4710,37 @@
       <c r="A3" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
       <c r="Y3" s="8"/>
       <c r="AA3" s="1"/>
     </row>
@@ -5481,37 +5485,37 @@
       <c r="A21" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="16" t="s">
+      <c r="N21" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
       <c r="S21" s="8"/>
-      <c r="T21" s="16" t="s">
+      <c r="T21" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="U21" s="17"/>
-      <c r="V21" s="17"/>
-      <c r="W21" s="17"/>
-      <c r="X21" s="17"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="21"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="21"/>
       <c r="Y21" s="8"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
@@ -6249,37 +6253,37 @@
       <c r="A38" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="16" t="s">
+      <c r="H38" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
       <c r="M38" s="8"/>
-      <c r="N38" s="16" t="s">
+      <c r="N38" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
-      <c r="Q38" s="17"/>
-      <c r="R38" s="17"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
       <c r="S38" s="8"/>
-      <c r="T38" s="16" t="s">
+      <c r="T38" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="U38" s="17"/>
-      <c r="V38" s="17"/>
-      <c r="W38" s="17"/>
-      <c r="X38" s="17"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="21"/>
+      <c r="X38" s="21"/>
       <c r="Y38" s="8"/>
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
@@ -7016,16 +7020,16 @@
       <c r="Y51" s="8"/>
     </row>
     <row r="55" spans="1:25" ht="19" x14ac:dyDescent="0.25">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="I55" s="22" t="s">
+      <c r="I55" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="J55" s="22"/>
+      <c r="J55" s="18"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="22" t="s">
         <v>236</v>
       </c>
       <c r="B56" s="7"/>
@@ -7046,7 +7050,7 @@
       <c r="Q56" s="7"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7">
@@ -7081,7 +7085,7 @@
       </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A58" s="18"/>
+      <c r="A58" s="22"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -7098,7 +7102,7 @@
       <c r="Q58" s="7"/>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A59" s="18"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -7115,7 +7119,7 @@
       <c r="Q59" s="7"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A60" s="18"/>
+      <c r="A60" s="22"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -7132,7 +7136,7 @@
       <c r="Q60" s="7"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A61" s="18"/>
+      <c r="A61" s="22"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
@@ -7149,7 +7153,7 @@
       <c r="Q61" s="7"/>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A62" s="18"/>
+      <c r="A62" s="22"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -7166,7 +7170,7 @@
       <c r="Q62" s="7"/>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A63" s="18"/>
+      <c r="A63" s="22"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -7183,7 +7187,7 @@
       <c r="Q63" s="7"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A64" s="18"/>
+      <c r="A64" s="22"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -7236,10 +7240,10 @@
       <c r="Q67" s="7"/>
     </row>
     <row r="71" spans="8:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="I71" s="22" t="s">
+      <c r="I71" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="J71" s="22"/>
+      <c r="J71" s="18"/>
     </row>
     <row r="72" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H72" s="19" t="s">
@@ -7400,10 +7404,10 @@
       <c r="Q83" s="7"/>
     </row>
     <row r="86" spans="6:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="I86" s="22" t="s">
+      <c r="I86" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="J86" s="22"/>
+      <c r="J86" s="18"/>
     </row>
     <row r="87" spans="6:19" x14ac:dyDescent="0.2">
       <c r="H87" s="19" t="s">
@@ -7579,26 +7583,26 @@
       <c r="Q98" s="7"/>
     </row>
     <row r="101" spans="8:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="I101" s="22" t="s">
+      <c r="I101" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="J101" s="22"/>
-      <c r="P101" s="22" t="s">
+      <c r="J101" s="18"/>
+      <c r="P101" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="Q101" s="22"/>
+      <c r="Q101" s="18"/>
     </row>
     <row r="102" spans="8:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
-      <c r="K102" s="20" t="s">
+      <c r="K102" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="L102" s="20"/>
-      <c r="P102" s="20" t="s">
+      <c r="L102" s="17"/>
+      <c r="P102" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="Q102" s="20"/>
+      <c r="Q102" s="17"/>
     </row>
     <row r="103" spans="8:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I103" s="7">
@@ -7606,190 +7610,200 @@
         <v>2060</v>
       </c>
       <c r="J103" s="7"/>
-      <c r="K103" s="20"/>
-      <c r="L103" s="20"/>
+      <c r="K103" s="17"/>
+      <c r="L103" s="17"/>
       <c r="O103">
         <f>MIN(O5,O12,O23,O30,O40,O47)</f>
         <v>2099</v>
       </c>
-      <c r="P103" s="20"/>
-      <c r="Q103" s="20"/>
+      <c r="P103" s="17"/>
+      <c r="Q103" s="17"/>
     </row>
     <row r="104" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
-      <c r="K104" s="20"/>
-      <c r="L104" s="20"/>
-      <c r="P104" s="20"/>
-      <c r="Q104" s="20"/>
+      <c r="K104" s="17"/>
+      <c r="L104" s="17"/>
+      <c r="P104" s="17"/>
+      <c r="Q104" s="17"/>
     </row>
     <row r="105" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
-      <c r="K105" s="20"/>
-      <c r="L105" s="20"/>
-      <c r="P105" s="20"/>
-      <c r="Q105" s="20"/>
+      <c r="K105" s="17"/>
+      <c r="L105" s="17"/>
+      <c r="P105" s="17"/>
+      <c r="Q105" s="17"/>
     </row>
     <row r="106" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
-      <c r="K106" s="20"/>
-      <c r="L106" s="20"/>
-      <c r="P106" s="20"/>
-      <c r="Q106" s="20"/>
+      <c r="K106" s="17"/>
+      <c r="L106" s="17"/>
+      <c r="P106" s="17"/>
+      <c r="Q106" s="17"/>
     </row>
     <row r="107" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
-      <c r="K107" s="20"/>
-      <c r="L107" s="20"/>
-      <c r="P107" s="20"/>
-      <c r="Q107" s="20"/>
+      <c r="K107" s="17"/>
+      <c r="L107" s="17"/>
+      <c r="P107" s="17"/>
+      <c r="Q107" s="17"/>
     </row>
     <row r="108" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
-      <c r="K108" s="20"/>
-      <c r="L108" s="20"/>
-      <c r="P108" s="20"/>
-      <c r="Q108" s="20"/>
+      <c r="K108" s="17"/>
+      <c r="L108" s="17"/>
+      <c r="P108" s="17"/>
+      <c r="Q108" s="17"/>
     </row>
     <row r="109" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
-      <c r="K109" s="20"/>
-      <c r="L109" s="20"/>
-      <c r="P109" s="20"/>
-      <c r="Q109" s="20"/>
+      <c r="K109" s="17"/>
+      <c r="L109" s="17"/>
+      <c r="P109" s="17"/>
+      <c r="Q109" s="17"/>
     </row>
     <row r="110" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
-      <c r="K110" s="20"/>
-      <c r="L110" s="20"/>
-      <c r="P110" s="20"/>
-      <c r="Q110" s="20"/>
+      <c r="K110" s="17"/>
+      <c r="L110" s="17"/>
+      <c r="P110" s="17"/>
+      <c r="Q110" s="17"/>
     </row>
     <row r="111" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
-      <c r="K111" s="20"/>
-      <c r="L111" s="20"/>
-      <c r="P111" s="20"/>
-      <c r="Q111" s="20"/>
+      <c r="K111" s="17"/>
+      <c r="L111" s="17"/>
+      <c r="P111" s="17"/>
+      <c r="Q111" s="17"/>
     </row>
     <row r="115" spans="15:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="P115" s="22" t="s">
+      <c r="P115" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="Q115" s="22"/>
+      <c r="Q115" s="18"/>
     </row>
     <row r="116" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P116" s="20" t="s">
+      <c r="P116" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="Q116" s="20"/>
+      <c r="Q116" s="17"/>
     </row>
     <row r="117" spans="15:17" x14ac:dyDescent="0.2">
       <c r="O117">
         <f>MIN(O6,O13,O24,O41,O48,O31)</f>
         <v>2088</v>
       </c>
-      <c r="P117" s="20"/>
-      <c r="Q117" s="20"/>
+      <c r="P117" s="17"/>
+      <c r="Q117" s="17"/>
     </row>
     <row r="118" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P118" s="20"/>
-      <c r="Q118" s="20"/>
+      <c r="P118" s="17"/>
+      <c r="Q118" s="17"/>
     </row>
     <row r="119" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P119" s="20"/>
-      <c r="Q119" s="20"/>
+      <c r="P119" s="17"/>
+      <c r="Q119" s="17"/>
     </row>
     <row r="120" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P120" s="20"/>
-      <c r="Q120" s="20"/>
+      <c r="P120" s="17"/>
+      <c r="Q120" s="17"/>
     </row>
     <row r="121" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P121" s="20"/>
-      <c r="Q121" s="20"/>
+      <c r="P121" s="17"/>
+      <c r="Q121" s="17"/>
     </row>
     <row r="122" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P122" s="20"/>
-      <c r="Q122" s="20"/>
+      <c r="P122" s="17"/>
+      <c r="Q122" s="17"/>
     </row>
     <row r="123" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P123" s="20"/>
-      <c r="Q123" s="20"/>
+      <c r="P123" s="17"/>
+      <c r="Q123" s="17"/>
     </row>
     <row r="124" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P124" s="20"/>
-      <c r="Q124" s="20"/>
+      <c r="P124" s="17"/>
+      <c r="Q124" s="17"/>
     </row>
     <row r="125" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P125" s="20"/>
-      <c r="Q125" s="20"/>
+      <c r="P125" s="17"/>
+      <c r="Q125" s="17"/>
     </row>
     <row r="128" spans="15:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="P128" s="22" t="s">
+      <c r="P128" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="Q128" s="22"/>
+      <c r="Q128" s="18"/>
     </row>
     <row r="129" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P129" s="20" t="s">
+      <c r="P129" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="Q129" s="20"/>
+      <c r="Q129" s="17"/>
     </row>
     <row r="130" spans="15:17" x14ac:dyDescent="0.2">
       <c r="O130">
         <f>MIN(O7,O14,O25,O32,O42,O49)</f>
         <v>2081</v>
       </c>
-      <c r="P130" s="20"/>
-      <c r="Q130" s="20"/>
+      <c r="P130" s="17"/>
+      <c r="Q130" s="17"/>
     </row>
     <row r="131" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P131" s="20"/>
-      <c r="Q131" s="20"/>
+      <c r="P131" s="17"/>
+      <c r="Q131" s="17"/>
     </row>
     <row r="132" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P132" s="20"/>
-      <c r="Q132" s="20"/>
+      <c r="P132" s="17"/>
+      <c r="Q132" s="17"/>
     </row>
     <row r="133" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P133" s="20"/>
-      <c r="Q133" s="20"/>
+      <c r="P133" s="17"/>
+      <c r="Q133" s="17"/>
     </row>
     <row r="134" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P134" s="20"/>
-      <c r="Q134" s="20"/>
+      <c r="P134" s="17"/>
+      <c r="Q134" s="17"/>
     </row>
     <row r="135" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P135" s="20"/>
-      <c r="Q135" s="20"/>
+      <c r="P135" s="17"/>
+      <c r="Q135" s="17"/>
     </row>
     <row r="136" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P136" s="20"/>
-      <c r="Q136" s="20"/>
+      <c r="P136" s="17"/>
+      <c r="Q136" s="17"/>
     </row>
     <row r="137" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P137" s="20"/>
-      <c r="Q137" s="20"/>
+      <c r="P137" s="17"/>
+      <c r="Q137" s="17"/>
     </row>
     <row r="138" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P138" s="20"/>
-      <c r="Q138" s="20"/>
+      <c r="P138" s="17"/>
+      <c r="Q138" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="K102:L111"/>
-    <mergeCell ref="P102:Q111"/>
-    <mergeCell ref="P115:Q115"/>
-    <mergeCell ref="P116:Q125"/>
-    <mergeCell ref="P128:Q128"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="N21:R21"/>
+    <mergeCell ref="T21:X21"/>
+    <mergeCell ref="A56:A64"/>
+    <mergeCell ref="H56:I67"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="N38:R38"/>
+    <mergeCell ref="T38:X38"/>
+    <mergeCell ref="I55:J55"/>
     <mergeCell ref="P129:Q138"/>
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="H72:I83"/>
@@ -7797,21 +7811,1597 @@
     <mergeCell ref="H87:I98"/>
     <mergeCell ref="I101:J101"/>
     <mergeCell ref="P101:Q101"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="N38:R38"/>
-    <mergeCell ref="T38:X38"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="A56:A64"/>
-    <mergeCell ref="H56:I67"/>
+    <mergeCell ref="K102:L111"/>
+    <mergeCell ref="P102:Q111"/>
+    <mergeCell ref="P115:Q115"/>
+    <mergeCell ref="P116:Q125"/>
+    <mergeCell ref="P128:Q128"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2340F614-5690-E04E-B7DB-263E8536FEDA}">
+  <dimension ref="A3:AC106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="T71" sqref="T71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="1.6640625" customWidth="1"/>
+    <col min="13" max="13" width="1.6640625" customWidth="1"/>
+    <col min="19" max="19" width="1.6640625" customWidth="1"/>
+    <col min="25" max="25" width="1.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="S4" s="8"/>
+      <c r="T4" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="X4" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2041</v>
+      </c>
+      <c r="C5" s="10">
+        <v>2028</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2032</v>
+      </c>
+      <c r="E5" s="10">
+        <v>2054</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2067</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="4">
+        <v>2128</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2076</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2091</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2207</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2301</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="4">
+        <v>2224</v>
+      </c>
+      <c r="O5" s="4">
+        <v>2122</v>
+      </c>
+      <c r="P5" s="4">
+        <v>2153</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>2301</v>
+      </c>
+      <c r="R5" s="4">
+        <v>2301</v>
+      </c>
+      <c r="S5" s="8"/>
+      <c r="T5" s="4">
+        <v>2301</v>
+      </c>
+      <c r="U5" s="4">
+        <v>2173</v>
+      </c>
+      <c r="V5" s="4">
+        <v>2228</v>
+      </c>
+      <c r="W5" s="4">
+        <v>2301</v>
+      </c>
+      <c r="X5" s="4">
+        <v>2301</v>
+      </c>
+      <c r="Y5" s="8"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2041</v>
+      </c>
+      <c r="C6" s="10">
+        <v>2028</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2032</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2052</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2061</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="4">
+        <v>2099</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2070</v>
+      </c>
+      <c r="J6" s="4">
+        <v>2082</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2145</v>
+      </c>
+      <c r="L6" s="4">
+        <v>2186</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="4">
+        <v>2166</v>
+      </c>
+      <c r="O6" s="4">
+        <v>2106</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2124</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>2252</v>
+      </c>
+      <c r="R6" s="4">
+        <v>2301</v>
+      </c>
+      <c r="S6" s="8"/>
+      <c r="T6" s="4">
+        <v>2228</v>
+      </c>
+      <c r="U6" s="4">
+        <v>2138</v>
+      </c>
+      <c r="V6" s="4">
+        <v>2164</v>
+      </c>
+      <c r="W6" s="4">
+        <v>2301</v>
+      </c>
+      <c r="X6" s="4">
+        <v>2301</v>
+      </c>
+      <c r="Y6" s="8"/>
+      <c r="AC6" s="1"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2041</v>
+      </c>
+      <c r="C7" s="10">
+        <v>2028</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2032</v>
+      </c>
+      <c r="E7" s="10">
+        <v>2052</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2059</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="4">
+        <v>2094</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2069</v>
+      </c>
+      <c r="J7" s="4">
+        <v>2078</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2121</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2141</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="4">
+        <v>2142</v>
+      </c>
+      <c r="O7" s="4">
+        <v>2098</v>
+      </c>
+      <c r="P7" s="4">
+        <v>2112</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>2189</v>
+      </c>
+      <c r="R7" s="4">
+        <v>2236</v>
+      </c>
+      <c r="S7" s="8"/>
+      <c r="T7" s="4">
+        <v>2185</v>
+      </c>
+      <c r="U7" s="4">
+        <v>2122</v>
+      </c>
+      <c r="V7" s="4">
+        <v>2140</v>
+      </c>
+      <c r="W7" s="4">
+        <v>2270</v>
+      </c>
+      <c r="X7" s="4">
+        <v>2301</v>
+      </c>
+      <c r="Y7" s="8"/>
+      <c r="AC7" s="2"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2039</v>
+      </c>
+      <c r="C8" s="10">
+        <v>2028</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2032</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2049</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2056</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="4">
+        <v>2088</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2065</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2073</v>
+      </c>
+      <c r="K8" s="4">
+        <v>2099</v>
+      </c>
+      <c r="L8" s="4">
+        <v>2128</v>
+      </c>
+      <c r="M8" s="8"/>
+      <c r="N8" s="4">
+        <v>2131</v>
+      </c>
+      <c r="O8" s="4">
+        <v>2092</v>
+      </c>
+      <c r="P8" s="4">
+        <v>2104</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>2173</v>
+      </c>
+      <c r="R8" s="4">
+        <v>2215</v>
+      </c>
+      <c r="S8" s="8"/>
+      <c r="T8" s="4">
+        <v>2173</v>
+      </c>
+      <c r="U8" s="4">
+        <v>2112</v>
+      </c>
+      <c r="V8" s="4">
+        <v>2129</v>
+      </c>
+      <c r="W8" s="4">
+        <v>2251</v>
+      </c>
+      <c r="X8" s="4">
+        <v>2301</v>
+      </c>
+      <c r="Y8" s="8"/>
+      <c r="AC8" s="4"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="G9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="AC9" s="4"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="G10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="AC10" s="4"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="S11" s="8"/>
+      <c r="T11" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="V11" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="W11" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="X11" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y11" s="8"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2040</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2027</v>
+      </c>
+      <c r="D12" s="10">
+        <v>2031</v>
+      </c>
+      <c r="E12" s="10">
+        <v>2054</v>
+      </c>
+      <c r="F12" s="10">
+        <v>2067</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="4">
+        <v>2123</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2067</v>
+      </c>
+      <c r="J12" s="4">
+        <v>2083</v>
+      </c>
+      <c r="K12" s="4">
+        <v>2207</v>
+      </c>
+      <c r="L12" s="4">
+        <v>2301</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="N12" s="4">
+        <v>2204</v>
+      </c>
+      <c r="O12" s="4">
+        <v>2099</v>
+      </c>
+      <c r="P12" s="4">
+        <v>2132</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>2301</v>
+      </c>
+      <c r="R12" s="4">
+        <v>2301</v>
+      </c>
+      <c r="S12" s="8"/>
+      <c r="T12" s="4">
+        <v>2275</v>
+      </c>
+      <c r="U12" s="4">
+        <v>2130</v>
+      </c>
+      <c r="V12" s="4">
+        <v>2176</v>
+      </c>
+      <c r="W12" s="4">
+        <v>2301</v>
+      </c>
+      <c r="X12" s="4">
+        <v>2301</v>
+      </c>
+      <c r="Y12" s="8"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2040</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2027</v>
+      </c>
+      <c r="D13" s="10">
+        <v>2031</v>
+      </c>
+      <c r="E13" s="10">
+        <v>2052</v>
+      </c>
+      <c r="F13" s="10">
+        <v>2061</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="4">
+        <v>2098</v>
+      </c>
+      <c r="I13" s="4">
+        <v>2063</v>
+      </c>
+      <c r="J13" s="4">
+        <v>2074</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2145</v>
+      </c>
+      <c r="L13" s="4">
+        <v>2186</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="4">
+        <v>2156</v>
+      </c>
+      <c r="O13" s="4">
+        <v>2088</v>
+      </c>
+      <c r="P13" s="4">
+        <v>2109</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>2252</v>
+      </c>
+      <c r="R13" s="4">
+        <v>2301</v>
+      </c>
+      <c r="S13" s="8"/>
+      <c r="T13" s="4">
+        <v>2210</v>
+      </c>
+      <c r="U13" s="4">
+        <v>2107</v>
+      </c>
+      <c r="V13" s="4">
+        <v>2126</v>
+      </c>
+      <c r="W13" s="4">
+        <v>2301</v>
+      </c>
+      <c r="X13" s="4">
+        <v>2301</v>
+      </c>
+      <c r="Y13" s="8"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2041</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2027</v>
+      </c>
+      <c r="D14" s="10">
+        <v>2031</v>
+      </c>
+      <c r="E14" s="10">
+        <v>2052</v>
+      </c>
+      <c r="F14" s="10">
+        <v>2059</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="4">
+        <v>2090</v>
+      </c>
+      <c r="I14" s="4">
+        <v>2060</v>
+      </c>
+      <c r="J14" s="4">
+        <v>2070</v>
+      </c>
+      <c r="K14" s="4">
+        <v>2121</v>
+      </c>
+      <c r="L14" s="4">
+        <v>2141</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="4">
+        <v>2130</v>
+      </c>
+      <c r="O14" s="4">
+        <v>2081</v>
+      </c>
+      <c r="P14" s="4">
+        <v>2098</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>2189</v>
+      </c>
+      <c r="R14" s="4">
+        <v>2236</v>
+      </c>
+      <c r="S14" s="8"/>
+      <c r="T14" s="4">
+        <v>2166</v>
+      </c>
+      <c r="U14" s="4">
+        <v>2097</v>
+      </c>
+      <c r="V14" s="4">
+        <v>2116</v>
+      </c>
+      <c r="W14" s="4">
+        <v>2270</v>
+      </c>
+      <c r="X14" s="4">
+        <v>2301</v>
+      </c>
+      <c r="Y14" s="8"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2039</v>
+      </c>
+      <c r="C15" s="10">
+        <v>2028</v>
+      </c>
+      <c r="D15" s="10">
+        <v>2031</v>
+      </c>
+      <c r="E15" s="10">
+        <v>2049</v>
+      </c>
+      <c r="F15" s="10">
+        <v>2056</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="4">
+        <v>2085</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2057</v>
+      </c>
+      <c r="J15" s="4">
+        <v>2066</v>
+      </c>
+      <c r="K15" s="4">
+        <v>2099</v>
+      </c>
+      <c r="L15" s="4">
+        <v>2128</v>
+      </c>
+      <c r="M15" s="8"/>
+      <c r="N15" s="4">
+        <v>2120</v>
+      </c>
+      <c r="O15" s="4">
+        <v>2076</v>
+      </c>
+      <c r="P15" s="4">
+        <v>2091</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>2173</v>
+      </c>
+      <c r="R15" s="4">
+        <v>2215</v>
+      </c>
+      <c r="S15" s="8"/>
+      <c r="T15" s="4">
+        <v>2154</v>
+      </c>
+      <c r="U15" s="4">
+        <v>2091</v>
+      </c>
+      <c r="V15" s="4">
+        <v>2112</v>
+      </c>
+      <c r="W15" s="4">
+        <v>2251</v>
+      </c>
+      <c r="X15" s="4">
+        <v>2301</v>
+      </c>
+      <c r="Y15" s="8"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="AB16" s="1"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB18" s="1"/>
+    </row>
+    <row r="19" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+    </row>
+    <row r="23" spans="1:28" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="J23" s="18"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="H24" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="I24" s="19"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A25" s="22"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7">
+        <f>MIN(D5:D7,D12:D14)</f>
+        <v>2031</v>
+      </c>
+      <c r="E25" s="7">
+        <f>MAX(E5:E7,E12:E14)</f>
+        <v>2054</v>
+      </c>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="11">
+        <v>2091</v>
+      </c>
+      <c r="K25" s="7">
+        <v>2207</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="11">
+        <v>2153</v>
+      </c>
+      <c r="Q25" s="11">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A26" s="22"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A27" s="22"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A28" s="22"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A29" s="22"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A30" s="22"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A31" s="22"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A32" s="22"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+    </row>
+    <row r="33" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+    </row>
+    <row r="34" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+    </row>
+    <row r="35" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+    </row>
+    <row r="39" spans="8:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="I39" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="J39" s="18"/>
+    </row>
+    <row r="40" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H40" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="I40" s="19"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+    </row>
+    <row r="41" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="11">
+        <v>2082</v>
+      </c>
+      <c r="K41" s="23">
+        <v>2145</v>
+      </c>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="11">
+        <v>2124</v>
+      </c>
+      <c r="Q41" s="13">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="42" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+    </row>
+    <row r="43" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+    </row>
+    <row r="44" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+    </row>
+    <row r="45" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+    </row>
+    <row r="46" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+    </row>
+    <row r="47" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+    </row>
+    <row r="48" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+    </row>
+    <row r="49" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+    </row>
+    <row r="50" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+    </row>
+    <row r="51" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+    </row>
+    <row r="54" spans="6:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="I54" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="J54" s="18"/>
+    </row>
+    <row r="55" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="H55" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="I55" s="19"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+    </row>
+    <row r="56" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="11">
+        <v>2078</v>
+      </c>
+      <c r="K56" s="11">
+        <v>2121</v>
+      </c>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="11">
+        <v>2112</v>
+      </c>
+      <c r="Q56" s="11">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="57" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+    </row>
+    <row r="58" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="S58" s="4"/>
+    </row>
+    <row r="59" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="S59" s="4"/>
+    </row>
+    <row r="60" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="S60" s="4"/>
+    </row>
+    <row r="61" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="F61" s="5"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="7"/>
+      <c r="P61" s="7"/>
+      <c r="Q61" s="7"/>
+      <c r="S61" s="4"/>
+    </row>
+    <row r="62" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="F62" s="5"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="7"/>
+      <c r="Q62" s="7"/>
+      <c r="S62" s="4"/>
+    </row>
+    <row r="63" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="7"/>
+      <c r="P63" s="7"/>
+      <c r="Q63" s="7"/>
+    </row>
+    <row r="64" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+    </row>
+    <row r="65" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
+      <c r="Q65" s="7"/>
+    </row>
+    <row r="66" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
+      <c r="N66" s="7"/>
+      <c r="O66" s="7"/>
+      <c r="P66" s="7"/>
+      <c r="Q66" s="7"/>
+    </row>
+    <row r="69" spans="8:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="I69" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="J69" s="18"/>
+      <c r="P69" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q69" s="18"/>
+    </row>
+    <row r="70" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="L70" s="17"/>
+      <c r="P70" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q70" s="17"/>
+    </row>
+    <row r="71" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="I71" s="7">
+        <f>MIN(I5:I7,I12:I14)</f>
+        <v>2060</v>
+      </c>
+      <c r="J71" s="7"/>
+      <c r="K71" s="17"/>
+      <c r="L71" s="17"/>
+      <c r="O71">
+        <f>MIN(O5,O12)</f>
+        <v>2099</v>
+      </c>
+      <c r="P71" s="17"/>
+      <c r="Q71" s="17"/>
+    </row>
+    <row r="72" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="17"/>
+      <c r="L72" s="17"/>
+      <c r="P72" s="17"/>
+      <c r="Q72" s="17"/>
+    </row>
+    <row r="73" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="17"/>
+      <c r="L73" s="17"/>
+      <c r="P73" s="17"/>
+      <c r="Q73" s="17"/>
+    </row>
+    <row r="74" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="17"/>
+      <c r="L74" s="17"/>
+      <c r="P74" s="17"/>
+      <c r="Q74" s="17"/>
+    </row>
+    <row r="75" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="17"/>
+      <c r="L75" s="17"/>
+      <c r="P75" s="17"/>
+      <c r="Q75" s="17"/>
+    </row>
+    <row r="76" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="17"/>
+      <c r="L76" s="17"/>
+      <c r="P76" s="17"/>
+      <c r="Q76" s="17"/>
+    </row>
+    <row r="77" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="17"/>
+      <c r="L77" s="17"/>
+      <c r="P77" s="17"/>
+      <c r="Q77" s="17"/>
+    </row>
+    <row r="78" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="17"/>
+      <c r="L78" s="17"/>
+      <c r="P78" s="17"/>
+      <c r="Q78" s="17"/>
+    </row>
+    <row r="79" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="17"/>
+      <c r="L79" s="17"/>
+      <c r="P79" s="17"/>
+      <c r="Q79" s="17"/>
+    </row>
+    <row r="83" spans="15:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="P83" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q83" s="18"/>
+    </row>
+    <row r="84" spans="15:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P84" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q84" s="17"/>
+    </row>
+    <row r="85" spans="15:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O85">
+        <f>MIN(O6,O13)</f>
+        <v>2088</v>
+      </c>
+      <c r="P85" s="17"/>
+      <c r="Q85" s="17"/>
+    </row>
+    <row r="86" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P86" s="17"/>
+      <c r="Q86" s="17"/>
+    </row>
+    <row r="87" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P87" s="17"/>
+      <c r="Q87" s="17"/>
+    </row>
+    <row r="88" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P88" s="17"/>
+      <c r="Q88" s="17"/>
+    </row>
+    <row r="89" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P89" s="17"/>
+      <c r="Q89" s="17"/>
+    </row>
+    <row r="90" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P90" s="17"/>
+      <c r="Q90" s="17"/>
+    </row>
+    <row r="91" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P91" s="17"/>
+      <c r="Q91" s="17"/>
+    </row>
+    <row r="92" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P92" s="17"/>
+      <c r="Q92" s="17"/>
+    </row>
+    <row r="93" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P93" s="17"/>
+      <c r="Q93" s="17"/>
+    </row>
+    <row r="96" spans="15:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="P96" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q96" s="18"/>
+    </row>
+    <row r="97" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P97" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q97" s="17"/>
+    </row>
+    <row r="98" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="O98">
+        <f>MIN(O7,O14)</f>
+        <v>2081</v>
+      </c>
+      <c r="P98" s="17"/>
+      <c r="Q98" s="17"/>
+    </row>
+    <row r="99" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P99" s="17"/>
+      <c r="Q99" s="17"/>
+    </row>
+    <row r="100" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P100" s="17"/>
+      <c r="Q100" s="17"/>
+    </row>
+    <row r="101" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P101" s="17"/>
+      <c r="Q101" s="17"/>
+    </row>
+    <row r="102" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P102" s="17"/>
+      <c r="Q102" s="17"/>
+    </row>
+    <row r="103" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P103" s="17"/>
+      <c r="Q103" s="17"/>
+    </row>
+    <row r="104" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P104" s="17"/>
+      <c r="Q104" s="17"/>
+    </row>
+    <row r="105" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P105" s="17"/>
+      <c r="Q105" s="17"/>
+    </row>
+    <row r="106" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="P106" s="17"/>
+      <c r="Q106" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="K70:L79"/>
+    <mergeCell ref="P70:Q79"/>
+    <mergeCell ref="P83:Q83"/>
+    <mergeCell ref="P84:Q93"/>
+    <mergeCell ref="P96:Q96"/>
+    <mergeCell ref="P97:Q106"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="H40:I51"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="H55:I66"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="P69:Q69"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="T3:X3"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="N21:R21"/>
-    <mergeCell ref="T21:X21"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="A24:A32"/>
+    <mergeCell ref="H24:I35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
:sparkles: round - round outward to the nearest half decade
</commit_message>
<xml_diff>
--- a/projects/2025_NJSTAP/Exceedance/tabulated/Exceedance_table_NJSTAP_praveen_new.xlsx
+++ b/projects/2025_NJSTAP/Exceedance/tabulated/Exceedance_table_NJSTAP_praveen_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/geekBoi_18/werk/amarel/scratch:pk695/NJ_STAP_report/notebooks/xcdance/_print.xcdance.table_xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E496600-C2AC-AE42-BF42-0C36328F42E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F703C1-7E22-2641-933D-0C874319CADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46840" yWindow="-18720" windowWidth="29920" windowHeight="18660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-46840" yWindow="-18720" windowWidth="34220" windowHeight="24320" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SANDY_HOOK" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="NYC" sheetId="6" r:id="rId4"/>
     <sheet name="Atlantic City" sheetId="2" r:id="rId5"/>
     <sheet name="NJSTAP.Coastal" sheetId="13" r:id="rId6"/>
-    <sheet name="NJSTAP_AtlanticCity" sheetId="14" r:id="rId7"/>
+    <sheet name="NJSTAP_AtlanticCity" sheetId="15" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="253">
   <si>
     <t>2042 (2027,2032, 2060,2081)</t>
   </si>
@@ -2878,13 +2878,16 @@
   </si>
   <si>
     <t>xls calculation 8</t>
+  </si>
+  <si>
+    <t>PLEASE NOTE: The data in BOLD enclosed in a box is rounded outward to the nearest half decade. We use =FLOOR(A1, 5)] for p&lt;50 ; and [=CEILING(B1, 5)] for p&gt;50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2939,8 +2942,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2965,8 +2976,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2974,11 +2991,132 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3018,15 +3156,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3034,9 +3163,62 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4710,37 +4892,37 @@
       <c r="A3" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="20" t="s">
+      <c r="T3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
       <c r="Y3" s="8"/>
       <c r="AA3" s="1"/>
     </row>
@@ -5485,37 +5667,37 @@
       <c r="A21" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="20" t="s">
+      <c r="N21" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
       <c r="S21" s="8"/>
-      <c r="T21" s="20" t="s">
+      <c r="T21" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="18"/>
       <c r="Y21" s="8"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
@@ -6253,37 +6435,37 @@
       <c r="A38" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="20" t="s">
+      <c r="H38" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
       <c r="M38" s="8"/>
-      <c r="N38" s="20" t="s">
+      <c r="N38" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="O38" s="21"/>
-      <c r="P38" s="21"/>
-      <c r="Q38" s="21"/>
-      <c r="R38" s="21"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
       <c r="S38" s="8"/>
-      <c r="T38" s="20" t="s">
+      <c r="T38" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="U38" s="21"/>
-      <c r="V38" s="21"/>
-      <c r="W38" s="21"/>
-      <c r="X38" s="21"/>
+      <c r="U38" s="18"/>
+      <c r="V38" s="18"/>
+      <c r="W38" s="18"/>
+      <c r="X38" s="18"/>
       <c r="Y38" s="8"/>
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
@@ -7023,23 +7205,23 @@
       <c r="A55" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="I55" s="18" t="s">
+      <c r="I55" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="J55" s="18"/>
+      <c r="J55" s="21"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="19" t="s">
         <v>236</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
-      <c r="H56" s="19" t="s">
+      <c r="H56" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="I56" s="19"/>
+      <c r="I56" s="20"/>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
@@ -7050,7 +7232,7 @@
       <c r="Q56" s="7"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A57" s="22"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7">
@@ -7061,8 +7243,8 @@
         <f>MAX(E5:E7,E12:E14,E23:E25,E30:E32,E40:E42,E47:E49)</f>
         <v>2056</v>
       </c>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
       <c r="J57" s="7">
         <f>MIN(J5,J23,J40)</f>
         <v>2091</v>
@@ -7085,13 +7267,13 @@
       </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A58" s="22"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
       <c r="L58" s="7"/>
@@ -7102,13 +7284,13 @@
       <c r="Q58" s="7"/>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A59" s="22"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
       <c r="L59" s="7"/>
@@ -7119,13 +7301,13 @@
       <c r="Q59" s="7"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A60" s="22"/>
+      <c r="A60" s="19"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
@@ -7136,13 +7318,13 @@
       <c r="Q60" s="7"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A61" s="22"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
@@ -7153,13 +7335,13 @@
       <c r="Q61" s="7"/>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A62" s="22"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
       <c r="L62" s="7"/>
@@ -7170,13 +7352,13 @@
       <c r="Q62" s="7"/>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A63" s="22"/>
+      <c r="A63" s="19"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
       <c r="L63" s="7"/>
@@ -7187,13 +7369,13 @@
       <c r="Q63" s="7"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A64" s="22"/>
+      <c r="A64" s="19"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
       <c r="L64" s="7"/>
@@ -7204,8 +7386,8 @@
       <c r="Q64" s="7"/>
     </row>
     <row r="65" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
       <c r="L65" s="7"/>
@@ -7216,8 +7398,8 @@
       <c r="Q65" s="7"/>
     </row>
     <row r="66" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
       <c r="L66" s="7"/>
@@ -7228,8 +7410,8 @@
       <c r="Q66" s="7"/>
     </row>
     <row r="67" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H67" s="19"/>
-      <c r="I67" s="19"/>
+      <c r="H67" s="20"/>
+      <c r="I67" s="20"/>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
       <c r="L67" s="7"/>
@@ -7240,16 +7422,16 @@
       <c r="Q67" s="7"/>
     </row>
     <row r="71" spans="8:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="I71" s="18" t="s">
+      <c r="I71" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="J71" s="18"/>
+      <c r="J71" s="21"/>
     </row>
     <row r="72" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H72" s="19" t="s">
+      <c r="H72" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="I72" s="19"/>
+      <c r="I72" s="20"/>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
@@ -7260,8 +7442,8 @@
       <c r="Q72" s="7"/>
     </row>
     <row r="73" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H73" s="19"/>
-      <c r="I73" s="19"/>
+      <c r="H73" s="20"/>
+      <c r="I73" s="20"/>
       <c r="J73" s="7">
         <f>MIN(J6,J24,J41)</f>
         <v>2082</v>
@@ -7284,8 +7466,8 @@
       </c>
     </row>
     <row r="74" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H74" s="19"/>
-      <c r="I74" s="19"/>
+      <c r="H74" s="20"/>
+      <c r="I74" s="20"/>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
@@ -7296,8 +7478,8 @@
       <c r="Q74" s="7"/>
     </row>
     <row r="75" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H75" s="19"/>
-      <c r="I75" s="19"/>
+      <c r="H75" s="20"/>
+      <c r="I75" s="20"/>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
@@ -7308,8 +7490,8 @@
       <c r="Q75" s="7"/>
     </row>
     <row r="76" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
+      <c r="H76" s="20"/>
+      <c r="I76" s="20"/>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
@@ -7320,8 +7502,8 @@
       <c r="Q76" s="7"/>
     </row>
     <row r="77" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H77" s="19"/>
-      <c r="I77" s="19"/>
+      <c r="H77" s="20"/>
+      <c r="I77" s="20"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
@@ -7332,8 +7514,8 @@
       <c r="Q77" s="7"/>
     </row>
     <row r="78" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H78" s="19"/>
-      <c r="I78" s="19"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="20"/>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
@@ -7344,8 +7526,8 @@
       <c r="Q78" s="7"/>
     </row>
     <row r="79" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H79" s="19"/>
-      <c r="I79" s="19"/>
+      <c r="H79" s="20"/>
+      <c r="I79" s="20"/>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
@@ -7356,8 +7538,8 @@
       <c r="Q79" s="7"/>
     </row>
     <row r="80" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H80" s="19"/>
-      <c r="I80" s="19"/>
+      <c r="H80" s="20"/>
+      <c r="I80" s="20"/>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
@@ -7368,8 +7550,8 @@
       <c r="Q80" s="7"/>
     </row>
     <row r="81" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H81" s="19"/>
-      <c r="I81" s="19"/>
+      <c r="H81" s="20"/>
+      <c r="I81" s="20"/>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
@@ -7380,8 +7562,8 @@
       <c r="Q81" s="7"/>
     </row>
     <row r="82" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H82" s="19"/>
-      <c r="I82" s="19"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="20"/>
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
       <c r="L82" s="7"/>
@@ -7392,8 +7574,8 @@
       <c r="Q82" s="7"/>
     </row>
     <row r="83" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H83" s="19"/>
-      <c r="I83" s="19"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="20"/>
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
       <c r="L83" s="7"/>
@@ -7404,16 +7586,16 @@
       <c r="Q83" s="7"/>
     </row>
     <row r="86" spans="6:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="I86" s="18" t="s">
+      <c r="I86" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="J86" s="18"/>
+      <c r="J86" s="21"/>
     </row>
     <row r="87" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H87" s="19" t="s">
+      <c r="H87" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="I87" s="19"/>
+      <c r="I87" s="20"/>
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
       <c r="L87" s="7"/>
@@ -7424,8 +7606,8 @@
       <c r="Q87" s="7"/>
     </row>
     <row r="88" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H88" s="19"/>
-      <c r="I88" s="19"/>
+      <c r="H88" s="20"/>
+      <c r="I88" s="20"/>
       <c r="J88" s="7">
         <f>MIN(J7,J25,J42)</f>
         <v>2078</v>
@@ -7448,8 +7630,8 @@
       </c>
     </row>
     <row r="89" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H89" s="19"/>
-      <c r="I89" s="19"/>
+      <c r="H89" s="20"/>
+      <c r="I89" s="20"/>
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
       <c r="L89" s="7"/>
@@ -7462,8 +7644,8 @@
     <row r="90" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
-      <c r="H90" s="19"/>
-      <c r="I90" s="19"/>
+      <c r="H90" s="20"/>
+      <c r="I90" s="20"/>
       <c r="J90" s="11"/>
       <c r="K90" s="7"/>
       <c r="L90" s="7"/>
@@ -7477,8 +7659,8 @@
     <row r="91" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
-      <c r="H91" s="19"/>
-      <c r="I91" s="19"/>
+      <c r="H91" s="20"/>
+      <c r="I91" s="20"/>
       <c r="J91" s="11"/>
       <c r="K91" s="7"/>
       <c r="L91" s="7"/>
@@ -7492,8 +7674,8 @@
     <row r="92" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
-      <c r="H92" s="19"/>
-      <c r="I92" s="19"/>
+      <c r="H92" s="20"/>
+      <c r="I92" s="20"/>
       <c r="J92" s="11"/>
       <c r="K92" s="7"/>
       <c r="L92" s="7"/>
@@ -7507,8 +7689,8 @@
     <row r="93" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F93" s="5"/>
       <c r="G93" s="4"/>
-      <c r="H93" s="19"/>
-      <c r="I93" s="19"/>
+      <c r="H93" s="20"/>
+      <c r="I93" s="20"/>
       <c r="J93" s="11"/>
       <c r="K93" s="7"/>
       <c r="L93" s="7"/>
@@ -7522,8 +7704,8 @@
     <row r="94" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F94" s="5"/>
       <c r="G94" s="4"/>
-      <c r="H94" s="19"/>
-      <c r="I94" s="19"/>
+      <c r="H94" s="20"/>
+      <c r="I94" s="20"/>
       <c r="J94" s="11"/>
       <c r="K94" s="7"/>
       <c r="L94" s="7"/>
@@ -7535,8 +7717,8 @@
       <c r="S94" s="4"/>
     </row>
     <row r="95" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H95" s="19"/>
-      <c r="I95" s="19"/>
+      <c r="H95" s="20"/>
+      <c r="I95" s="20"/>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
       <c r="L95" s="7"/>
@@ -7547,8 +7729,8 @@
       <c r="Q95" s="7"/>
     </row>
     <row r="96" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H96" s="19"/>
-      <c r="I96" s="19"/>
+      <c r="H96" s="20"/>
+      <c r="I96" s="20"/>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
       <c r="L96" s="7"/>
@@ -7559,8 +7741,8 @@
       <c r="Q96" s="7"/>
     </row>
     <row r="97" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H97" s="19"/>
-      <c r="I97" s="19"/>
+      <c r="H97" s="20"/>
+      <c r="I97" s="20"/>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
       <c r="L97" s="7"/>
@@ -7571,8 +7753,8 @@
       <c r="Q97" s="7"/>
     </row>
     <row r="98" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H98" s="19"/>
-      <c r="I98" s="19"/>
+      <c r="H98" s="20"/>
+      <c r="I98" s="20"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
       <c r="L98" s="7"/>
@@ -7583,26 +7765,26 @@
       <c r="Q98" s="7"/>
     </row>
     <row r="101" spans="8:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="I101" s="18" t="s">
+      <c r="I101" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="J101" s="18"/>
-      <c r="P101" s="18" t="s">
+      <c r="J101" s="21"/>
+      <c r="P101" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="Q101" s="18"/>
+      <c r="Q101" s="21"/>
     </row>
     <row r="102" spans="8:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
-      <c r="K102" s="17" t="s">
+      <c r="K102" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="L102" s="17"/>
-      <c r="P102" s="17" t="s">
+      <c r="L102" s="22"/>
+      <c r="P102" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="Q102" s="17"/>
+      <c r="Q102" s="22"/>
     </row>
     <row r="103" spans="8:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I103" s="7">
@@ -7610,198 +7792,185 @@
         <v>2060</v>
       </c>
       <c r="J103" s="7"/>
-      <c r="K103" s="17"/>
-      <c r="L103" s="17"/>
+      <c r="K103" s="22"/>
+      <c r="L103" s="22"/>
       <c r="O103">
         <f>MIN(O5,O12,O23,O30,O40,O47)</f>
         <v>2099</v>
       </c>
-      <c r="P103" s="17"/>
-      <c r="Q103" s="17"/>
+      <c r="P103" s="22"/>
+      <c r="Q103" s="22"/>
     </row>
     <row r="104" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
-      <c r="K104" s="17"/>
-      <c r="L104" s="17"/>
-      <c r="P104" s="17"/>
-      <c r="Q104" s="17"/>
+      <c r="K104" s="22"/>
+      <c r="L104" s="22"/>
+      <c r="P104" s="22"/>
+      <c r="Q104" s="22"/>
     </row>
     <row r="105" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
-      <c r="K105" s="17"/>
-      <c r="L105" s="17"/>
-      <c r="P105" s="17"/>
-      <c r="Q105" s="17"/>
+      <c r="K105" s="22"/>
+      <c r="L105" s="22"/>
+      <c r="P105" s="22"/>
+      <c r="Q105" s="22"/>
     </row>
     <row r="106" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
-      <c r="K106" s="17"/>
-      <c r="L106" s="17"/>
-      <c r="P106" s="17"/>
-      <c r="Q106" s="17"/>
+      <c r="K106" s="22"/>
+      <c r="L106" s="22"/>
+      <c r="P106" s="22"/>
+      <c r="Q106" s="22"/>
     </row>
     <row r="107" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
-      <c r="K107" s="17"/>
-      <c r="L107" s="17"/>
-      <c r="P107" s="17"/>
-      <c r="Q107" s="17"/>
+      <c r="K107" s="22"/>
+      <c r="L107" s="22"/>
+      <c r="P107" s="22"/>
+      <c r="Q107" s="22"/>
     </row>
     <row r="108" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
-      <c r="K108" s="17"/>
-      <c r="L108" s="17"/>
-      <c r="P108" s="17"/>
-      <c r="Q108" s="17"/>
+      <c r="K108" s="22"/>
+      <c r="L108" s="22"/>
+      <c r="P108" s="22"/>
+      <c r="Q108" s="22"/>
     </row>
     <row r="109" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
-      <c r="K109" s="17"/>
-      <c r="L109" s="17"/>
-      <c r="P109" s="17"/>
-      <c r="Q109" s="17"/>
+      <c r="K109" s="22"/>
+      <c r="L109" s="22"/>
+      <c r="P109" s="22"/>
+      <c r="Q109" s="22"/>
     </row>
     <row r="110" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
-      <c r="K110" s="17"/>
-      <c r="L110" s="17"/>
-      <c r="P110" s="17"/>
-      <c r="Q110" s="17"/>
+      <c r="K110" s="22"/>
+      <c r="L110" s="22"/>
+      <c r="P110" s="22"/>
+      <c r="Q110" s="22"/>
     </row>
     <row r="111" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
-      <c r="K111" s="17"/>
-      <c r="L111" s="17"/>
-      <c r="P111" s="17"/>
-      <c r="Q111" s="17"/>
+      <c r="K111" s="22"/>
+      <c r="L111" s="22"/>
+      <c r="P111" s="22"/>
+      <c r="Q111" s="22"/>
     </row>
     <row r="115" spans="15:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="P115" s="18" t="s">
+      <c r="P115" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="Q115" s="18"/>
+      <c r="Q115" s="21"/>
     </row>
     <row r="116" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P116" s="17" t="s">
+      <c r="P116" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="Q116" s="17"/>
+      <c r="Q116" s="22"/>
     </row>
     <row r="117" spans="15:17" x14ac:dyDescent="0.2">
       <c r="O117">
         <f>MIN(O6,O13,O24,O41,O48,O31)</f>
         <v>2088</v>
       </c>
-      <c r="P117" s="17"/>
-      <c r="Q117" s="17"/>
+      <c r="P117" s="22"/>
+      <c r="Q117" s="22"/>
     </row>
     <row r="118" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P118" s="17"/>
-      <c r="Q118" s="17"/>
+      <c r="P118" s="22"/>
+      <c r="Q118" s="22"/>
     </row>
     <row r="119" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P119" s="17"/>
-      <c r="Q119" s="17"/>
+      <c r="P119" s="22"/>
+      <c r="Q119" s="22"/>
     </row>
     <row r="120" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P120" s="17"/>
-      <c r="Q120" s="17"/>
+      <c r="P120" s="22"/>
+      <c r="Q120" s="22"/>
     </row>
     <row r="121" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P121" s="17"/>
-      <c r="Q121" s="17"/>
+      <c r="P121" s="22"/>
+      <c r="Q121" s="22"/>
     </row>
     <row r="122" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P122" s="17"/>
-      <c r="Q122" s="17"/>
+      <c r="P122" s="22"/>
+      <c r="Q122" s="22"/>
     </row>
     <row r="123" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P123" s="17"/>
-      <c r="Q123" s="17"/>
+      <c r="P123" s="22"/>
+      <c r="Q123" s="22"/>
     </row>
     <row r="124" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P124" s="17"/>
-      <c r="Q124" s="17"/>
+      <c r="P124" s="22"/>
+      <c r="Q124" s="22"/>
     </row>
     <row r="125" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P125" s="17"/>
-      <c r="Q125" s="17"/>
+      <c r="P125" s="22"/>
+      <c r="Q125" s="22"/>
     </row>
     <row r="128" spans="15:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="P128" s="18" t="s">
+      <c r="P128" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="Q128" s="18"/>
+      <c r="Q128" s="21"/>
     </row>
     <row r="129" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P129" s="17" t="s">
+      <c r="P129" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="Q129" s="17"/>
+      <c r="Q129" s="22"/>
     </row>
     <row r="130" spans="15:17" x14ac:dyDescent="0.2">
       <c r="O130">
         <f>MIN(O7,O14,O25,O32,O42,O49)</f>
         <v>2081</v>
       </c>
-      <c r="P130" s="17"/>
-      <c r="Q130" s="17"/>
+      <c r="P130" s="22"/>
+      <c r="Q130" s="22"/>
     </row>
     <row r="131" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P131" s="17"/>
-      <c r="Q131" s="17"/>
+      <c r="P131" s="22"/>
+      <c r="Q131" s="22"/>
     </row>
     <row r="132" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P132" s="17"/>
-      <c r="Q132" s="17"/>
+      <c r="P132" s="22"/>
+      <c r="Q132" s="22"/>
     </row>
     <row r="133" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P133" s="17"/>
-      <c r="Q133" s="17"/>
+      <c r="P133" s="22"/>
+      <c r="Q133" s="22"/>
     </row>
     <row r="134" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P134" s="17"/>
-      <c r="Q134" s="17"/>
+      <c r="P134" s="22"/>
+      <c r="Q134" s="22"/>
     </row>
     <row r="135" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P135" s="17"/>
-      <c r="Q135" s="17"/>
+      <c r="P135" s="22"/>
+      <c r="Q135" s="22"/>
     </row>
     <row r="136" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P136" s="17"/>
-      <c r="Q136" s="17"/>
+      <c r="P136" s="22"/>
+      <c r="Q136" s="22"/>
     </row>
     <row r="137" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P137" s="17"/>
-      <c r="Q137" s="17"/>
+      <c r="P137" s="22"/>
+      <c r="Q137" s="22"/>
     </row>
     <row r="138" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P138" s="17"/>
-      <c r="Q138" s="17"/>
+      <c r="P138" s="22"/>
+      <c r="Q138" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="N21:R21"/>
-    <mergeCell ref="T21:X21"/>
-    <mergeCell ref="A56:A64"/>
-    <mergeCell ref="H56:I67"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="N38:R38"/>
     <mergeCell ref="T38:X38"/>
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="P129:Q138"/>
@@ -7816,17 +7985,30 @@
     <mergeCell ref="P115:Q115"/>
     <mergeCell ref="P116:Q125"/>
     <mergeCell ref="P128:Q128"/>
+    <mergeCell ref="A56:A64"/>
+    <mergeCell ref="H56:I67"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="N38:R38"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="N21:R21"/>
+    <mergeCell ref="T21:X21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2340F614-5690-E04E-B7DB-263E8536FEDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42D21C4-B45D-3048-8C06-BA7A274B49E3}">
   <dimension ref="A3:AC106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="T71" sqref="T71"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7844,40 +8026,40 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="41" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="20" t="s">
+      <c r="T3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
       <c r="Y3" s="8"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -8627,23 +8809,23 @@
       <c r="A23" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="I23" s="18" t="s">
+      <c r="I23" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="J23" s="18"/>
+      <c r="J23" s="21"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="19" t="s">
         <v>236</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="I24" s="19"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -8654,7 +8836,7 @@
       <c r="Q24" s="7"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7">
@@ -8665,8 +8847,8 @@
         <f>MAX(E5:E7,E12:E14)</f>
         <v>2054</v>
       </c>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="11">
         <v>2091</v>
       </c>
@@ -8684,14 +8866,14 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
+    <row r="26" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
@@ -8703,31 +8885,49 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
+    <row r="27" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
+      <c r="D27" s="23">
+        <f>FLOOR(D25,5)</f>
+        <v>2030</v>
+      </c>
+      <c r="E27" s="24">
+        <f>CEILING(E25, 5)</f>
+        <v>2055</v>
+      </c>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="25">
+        <f>FLOOR(J25,5)</f>
+        <v>2090</v>
+      </c>
+      <c r="K27" s="24">
+        <f>CEILING(K25, 5)</f>
+        <v>2210</v>
+      </c>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
+      <c r="P27" s="9">
+        <f>FLOOR(P25,5)</f>
+        <v>2150</v>
+      </c>
+      <c r="Q27" s="11">
+        <f>CEILING(Q25, 5)</f>
+        <v>2305</v>
+      </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
@@ -8738,13 +8938,13 @@
       <c r="Q28" s="7"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A29" s="22"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
@@ -8755,13 +8955,13 @@
       <c r="Q29" s="7"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A30" s="22"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
@@ -8772,13 +8972,13 @@
       <c r="Q30" s="7"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A31" s="22"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
@@ -8789,13 +8989,13 @@
       <c r="Q31" s="7"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A32" s="22"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
@@ -8805,9 +9005,9 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
@@ -8817,9 +9017,9 @@
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
     </row>
-    <row r="34" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
@@ -8829,9 +9029,9 @@
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
     </row>
-    <row r="35" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
@@ -8841,17 +9041,34 @@
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
     </row>
-    <row r="39" spans="8:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="I39" s="18" t="s">
+    <row r="37" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="28"/>
+    </row>
+    <row r="39" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="29"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="31"/>
+      <c r="I39" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="J39" s="18"/>
-    </row>
-    <row r="40" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H40" s="19" t="s">
+      <c r="J39" s="21"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="29"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
+      <c r="H40" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="I40" s="19"/>
+      <c r="I40" s="20"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
@@ -8861,13 +9078,17 @@
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
     </row>
-    <row r="41" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="29"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="31"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
       <c r="J41" s="11">
         <v>2082</v>
       </c>
-      <c r="K41" s="23">
+      <c r="K41" s="11">
         <v>2145</v>
       </c>
       <c r="L41" s="7"/>
@@ -8877,13 +9098,17 @@
       <c r="P41" s="11">
         <v>2124</v>
       </c>
-      <c r="Q41" s="13">
+      <c r="Q41" s="7">
         <v>2252</v>
       </c>
     </row>
-    <row r="42" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
+    <row r="42" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="29"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="31"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
       <c r="L42" s="7"/>
@@ -8893,21 +9118,41 @@
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
     </row>
-    <row r="43" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
+    <row r="43" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="29"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="31"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="25">
+        <f>FLOOR(J41,5)</f>
+        <v>2080</v>
+      </c>
+      <c r="K43" s="32">
+        <f>CEILING(K41, 5)</f>
+        <v>2145</v>
+      </c>
       <c r="L43" s="7"/>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
       <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-    </row>
-    <row r="44" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
+      <c r="P43" s="33">
+        <f>FLOOR(P41,5)</f>
+        <v>2120</v>
+      </c>
+      <c r="Q43" s="34">
+        <f>CEILING(Q41, 5)</f>
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="35"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="37"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
@@ -8917,9 +9162,9 @@
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
     </row>
-    <row r="45" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
@@ -8929,9 +9174,9 @@
       <c r="P45" s="7"/>
       <c r="Q45" s="7"/>
     </row>
-    <row r="46" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
@@ -8941,9 +9186,9 @@
       <c r="P46" s="7"/>
       <c r="Q46" s="7"/>
     </row>
-    <row r="47" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
       <c r="L47" s="7"/>
@@ -8953,9 +9198,9 @@
       <c r="P47" s="7"/>
       <c r="Q47" s="7"/>
     </row>
-    <row r="48" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
@@ -8966,8 +9211,8 @@
       <c r="Q48" s="7"/>
     </row>
     <row r="49" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
       <c r="L49" s="7"/>
@@ -8978,8 +9223,8 @@
       <c r="Q49" s="7"/>
     </row>
     <row r="50" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
@@ -8990,8 +9235,8 @@
       <c r="Q50" s="7"/>
     </row>
     <row r="51" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
       <c r="L51" s="7"/>
@@ -9002,16 +9247,16 @@
       <c r="Q51" s="7"/>
     </row>
     <row r="54" spans="6:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="I54" s="18" t="s">
+      <c r="I54" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="J54" s="18"/>
+      <c r="J54" s="21"/>
     </row>
     <row r="55" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H55" s="19" t="s">
+      <c r="H55" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="I55" s="19"/>
+      <c r="I55" s="20"/>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
       <c r="L55" s="7"/>
@@ -9022,8 +9267,8 @@
       <c r="Q55" s="7"/>
     </row>
     <row r="56" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
       <c r="J56" s="11">
         <v>2078</v>
       </c>
@@ -9041,9 +9286,9 @@
         <v>2189</v>
       </c>
     </row>
-    <row r="57" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
+    <row r="57" spans="6:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
       <c r="L57" s="7"/>
@@ -9053,13 +9298,19 @@
       <c r="P57" s="7"/>
       <c r="Q57" s="7"/>
     </row>
-    <row r="58" spans="6:19" x14ac:dyDescent="0.2">
+    <row r="58" spans="6:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="7"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="38">
+        <f>FLOOR(J56,5)</f>
+        <v>2075</v>
+      </c>
+      <c r="K58" s="39">
+        <f>CEILING(K56, 5)</f>
+        <v>2125</v>
+      </c>
       <c r="L58" s="7"/>
       <c r="M58" s="11"/>
       <c r="N58" s="7"/>
@@ -9068,26 +9319,32 @@
       <c r="Q58" s="7"/>
       <c r="S58" s="4"/>
     </row>
-    <row r="59" spans="6:19" x14ac:dyDescent="0.2">
+    <row r="59" spans="6:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
       <c r="J59" s="11"/>
       <c r="K59" s="7"/>
       <c r="L59" s="7"/>
       <c r="M59" s="11"/>
       <c r="N59" s="7"/>
       <c r="O59" s="7"/>
-      <c r="P59" s="7"/>
-      <c r="Q59" s="7"/>
+      <c r="P59" s="25">
+        <f>FLOOR(P56,5)</f>
+        <v>2110</v>
+      </c>
+      <c r="Q59" s="24">
+        <f>CEILING(Q56, 5)</f>
+        <v>2190</v>
+      </c>
       <c r="S59" s="4"/>
     </row>
     <row r="60" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
       <c r="J60" s="11"/>
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
@@ -9101,8 +9358,8 @@
     <row r="61" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F61" s="5"/>
       <c r="G61" s="4"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
       <c r="J61" s="11"/>
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
@@ -9116,8 +9373,8 @@
     <row r="62" spans="6:19" x14ac:dyDescent="0.2">
       <c r="F62" s="5"/>
       <c r="G62" s="4"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
       <c r="J62" s="11"/>
       <c r="K62" s="7"/>
       <c r="L62" s="7"/>
@@ -9129,8 +9386,8 @@
       <c r="S62" s="4"/>
     </row>
     <row r="63" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
       <c r="L63" s="7"/>
@@ -9141,8 +9398,8 @@
       <c r="Q63" s="7"/>
     </row>
     <row r="64" spans="6:19" x14ac:dyDescent="0.2">
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
       <c r="L64" s="7"/>
@@ -9153,8 +9410,8 @@
       <c r="Q64" s="7"/>
     </row>
     <row r="65" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
       <c r="L65" s="7"/>
@@ -9165,8 +9422,8 @@
       <c r="Q65" s="7"/>
     </row>
     <row r="66" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
       <c r="L66" s="7"/>
@@ -9177,26 +9434,26 @@
       <c r="Q66" s="7"/>
     </row>
     <row r="69" spans="8:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="I69" s="18" t="s">
+      <c r="I69" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="J69" s="18"/>
-      <c r="P69" s="18" t="s">
+      <c r="J69" s="21"/>
+      <c r="P69" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="Q69" s="18"/>
+      <c r="Q69" s="21"/>
     </row>
     <row r="70" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
-      <c r="K70" s="17" t="s">
+      <c r="K70" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="L70" s="17"/>
-      <c r="P70" s="17" t="s">
+      <c r="L70" s="22"/>
+      <c r="P70" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="Q70" s="17"/>
+      <c r="Q70" s="22"/>
     </row>
     <row r="71" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I71" s="7">
@@ -9204,197 +9461,210 @@
         <v>2060</v>
       </c>
       <c r="J71" s="7"/>
-      <c r="K71" s="17"/>
-      <c r="L71" s="17"/>
+      <c r="K71" s="22"/>
+      <c r="L71" s="22"/>
       <c r="O71">
         <f>MIN(O5,O12)</f>
         <v>2099</v>
       </c>
-      <c r="P71" s="17"/>
-      <c r="Q71" s="17"/>
-    </row>
-    <row r="72" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="P71" s="22"/>
+      <c r="Q71" s="22"/>
+    </row>
+    <row r="72" spans="8:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
-      <c r="K72" s="17"/>
-      <c r="L72" s="17"/>
-      <c r="P72" s="17"/>
-      <c r="Q72" s="17"/>
-    </row>
-    <row r="73" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="K72" s="22"/>
+      <c r="L72" s="22"/>
+      <c r="P72" s="22"/>
+      <c r="Q72" s="22"/>
+    </row>
+    <row r="73" spans="8:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
-      <c r="K73" s="17"/>
-      <c r="L73" s="17"/>
-      <c r="P73" s="17"/>
-      <c r="Q73" s="17"/>
+      <c r="K73" s="22"/>
+      <c r="L73" s="22"/>
+      <c r="O73" s="40">
+        <f>FLOOR(O71,5)</f>
+        <v>2095</v>
+      </c>
+      <c r="P73" s="22"/>
+      <c r="Q73" s="22"/>
     </row>
     <row r="74" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
-      <c r="K74" s="17"/>
-      <c r="L74" s="17"/>
-      <c r="P74" s="17"/>
-      <c r="Q74" s="17"/>
+      <c r="K74" s="22"/>
+      <c r="L74" s="22"/>
+      <c r="P74" s="22"/>
+      <c r="Q74" s="22"/>
     </row>
     <row r="75" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
-      <c r="K75" s="17"/>
-      <c r="L75" s="17"/>
-      <c r="P75" s="17"/>
-      <c r="Q75" s="17"/>
+      <c r="K75" s="22"/>
+      <c r="L75" s="22"/>
+      <c r="P75" s="22"/>
+      <c r="Q75" s="22"/>
     </row>
     <row r="76" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
-      <c r="K76" s="17"/>
-      <c r="L76" s="17"/>
-      <c r="P76" s="17"/>
-      <c r="Q76" s="17"/>
+      <c r="K76" s="22"/>
+      <c r="L76" s="22"/>
+      <c r="P76" s="22"/>
+      <c r="Q76" s="22"/>
     </row>
     <row r="77" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
-      <c r="K77" s="17"/>
-      <c r="L77" s="17"/>
-      <c r="P77" s="17"/>
-      <c r="Q77" s="17"/>
+      <c r="K77" s="22"/>
+      <c r="L77" s="22"/>
+      <c r="P77" s="22"/>
+      <c r="Q77" s="22"/>
     </row>
     <row r="78" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
-      <c r="K78" s="17"/>
-      <c r="L78" s="17"/>
-      <c r="P78" s="17"/>
-      <c r="Q78" s="17"/>
+      <c r="K78" s="22"/>
+      <c r="L78" s="22"/>
+      <c r="P78" s="22"/>
+      <c r="Q78" s="22"/>
     </row>
     <row r="79" spans="8:17" x14ac:dyDescent="0.2">
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
-      <c r="K79" s="17"/>
-      <c r="L79" s="17"/>
-      <c r="P79" s="17"/>
-      <c r="Q79" s="17"/>
+      <c r="K79" s="22"/>
+      <c r="L79" s="22"/>
+      <c r="P79" s="22"/>
+      <c r="Q79" s="22"/>
     </row>
     <row r="83" spans="15:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="P83" s="18" t="s">
+      <c r="P83" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="Q83" s="18"/>
+      <c r="Q83" s="21"/>
     </row>
     <row r="84" spans="15:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P84" s="17" t="s">
+      <c r="P84" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="Q84" s="17"/>
+      <c r="Q84" s="22"/>
     </row>
     <row r="85" spans="15:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O85">
         <f>MIN(O6,O13)</f>
         <v>2088</v>
       </c>
-      <c r="P85" s="17"/>
-      <c r="Q85" s="17"/>
-    </row>
-    <row r="86" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P86" s="17"/>
-      <c r="Q86" s="17"/>
-    </row>
-    <row r="87" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P87" s="17"/>
-      <c r="Q87" s="17"/>
+      <c r="P85" s="22"/>
+      <c r="Q85" s="22"/>
+    </row>
+    <row r="86" spans="15:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P86" s="22"/>
+      <c r="Q86" s="22"/>
+    </row>
+    <row r="87" spans="15:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O87" s="40">
+        <f>FLOOR(O85,5)</f>
+        <v>2085</v>
+      </c>
+      <c r="P87" s="22"/>
+      <c r="Q87" s="22"/>
     </row>
     <row r="88" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P88" s="17"/>
-      <c r="Q88" s="17"/>
+      <c r="P88" s="22"/>
+      <c r="Q88" s="22"/>
     </row>
     <row r="89" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P89" s="17"/>
-      <c r="Q89" s="17"/>
+      <c r="P89" s="22"/>
+      <c r="Q89" s="22"/>
     </row>
     <row r="90" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P90" s="17"/>
-      <c r="Q90" s="17"/>
+      <c r="P90" s="22"/>
+      <c r="Q90" s="22"/>
     </row>
     <row r="91" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P91" s="17"/>
-      <c r="Q91" s="17"/>
+      <c r="P91" s="22"/>
+      <c r="Q91" s="22"/>
     </row>
     <row r="92" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P92" s="17"/>
-      <c r="Q92" s="17"/>
+      <c r="P92" s="22"/>
+      <c r="Q92" s="22"/>
     </row>
     <row r="93" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P93" s="17"/>
-      <c r="Q93" s="17"/>
+      <c r="P93" s="22"/>
+      <c r="Q93" s="22"/>
     </row>
     <row r="96" spans="15:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="P96" s="18" t="s">
+      <c r="P96" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="Q96" s="18"/>
+      <c r="Q96" s="21"/>
     </row>
     <row r="97" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P97" s="17" t="s">
+      <c r="P97" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="Q97" s="17"/>
+      <c r="Q97" s="22"/>
     </row>
     <row r="98" spans="15:17" x14ac:dyDescent="0.2">
       <c r="O98">
         <f>MIN(O7,O14)</f>
         <v>2081</v>
       </c>
-      <c r="P98" s="17"/>
-      <c r="Q98" s="17"/>
-    </row>
-    <row r="99" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P99" s="17"/>
-      <c r="Q99" s="17"/>
-    </row>
-    <row r="100" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P100" s="17"/>
-      <c r="Q100" s="17"/>
+      <c r="P98" s="22"/>
+      <c r="Q98" s="22"/>
+    </row>
+    <row r="99" spans="15:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P99" s="22"/>
+      <c r="Q99" s="22"/>
+    </row>
+    <row r="100" spans="15:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O100" s="40">
+        <f>FLOOR(O98,5)</f>
+        <v>2080</v>
+      </c>
+      <c r="P100" s="22"/>
+      <c r="Q100" s="22"/>
     </row>
     <row r="101" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P101" s="17"/>
-      <c r="Q101" s="17"/>
+      <c r="P101" s="22"/>
+      <c r="Q101" s="22"/>
     </row>
     <row r="102" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P102" s="17"/>
-      <c r="Q102" s="17"/>
+      <c r="P102" s="22"/>
+      <c r="Q102" s="22"/>
     </row>
     <row r="103" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P103" s="17"/>
-      <c r="Q103" s="17"/>
+      <c r="P103" s="22"/>
+      <c r="Q103" s="22"/>
     </row>
     <row r="104" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P104" s="17"/>
-      <c r="Q104" s="17"/>
+      <c r="P104" s="22"/>
+      <c r="Q104" s="22"/>
     </row>
     <row r="105" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P105" s="17"/>
-      <c r="Q105" s="17"/>
+      <c r="P105" s="22"/>
+      <c r="Q105" s="22"/>
     </row>
     <row r="106" spans="15:17" x14ac:dyDescent="0.2">
-      <c r="P106" s="17"/>
-      <c r="Q106" s="17"/>
+      <c r="P106" s="22"/>
+      <c r="Q106" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
+    <mergeCell ref="P97:Q106"/>
+    <mergeCell ref="P69:Q69"/>
     <mergeCell ref="K70:L79"/>
     <mergeCell ref="P70:Q79"/>
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P84:Q93"/>
     <mergeCell ref="P96:Q96"/>
-    <mergeCell ref="P97:Q106"/>
+    <mergeCell ref="A38:D44"/>
     <mergeCell ref="I39:J39"/>
     <mergeCell ref="H40:I51"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="H55:I66"/>
     <mergeCell ref="I69:J69"/>
-    <mergeCell ref="P69:Q69"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="N3:R3"/>

</xml_diff>